<commit_message>
user stories spreadsheet updated to reflect completion of payment system
</commit_message>
<xml_diff>
--- a/documentation/user_stories_models_v2.xlsx
+++ b/documentation/user_stories_models_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\608868804\OneDrive - BT Plc\Documents\Code_Institute\Milestone_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9C7A4D55-595F-4FD9-88A1-1BE0D79DBBFF}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E5ABE539-CE02-4125-BDBB-2E90B539A751}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
   </bookViews>
   <sheets>
     <sheet name="User_Stories" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
   <si>
     <t>User Story ID</t>
   </si>
@@ -369,6 +369,15 @@
   </si>
   <si>
     <t>Compelte</t>
+  </si>
+  <si>
+    <t>Complete  - Bag app</t>
+  </si>
+  <si>
+    <t>Edit Shipping cost per country/continent</t>
+  </si>
+  <si>
+    <t>Option to change shipping cost depending on the location of the customer</t>
   </si>
 </sst>
 </file>
@@ -421,7 +430,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +463,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,7 +586,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -585,6 +600,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,6 +616,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -610,9 +629,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -933,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C557C4-B67B-4897-99C4-67C9935146BD}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,13 +963,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -973,13 +989,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -1067,13 +1083,13 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
@@ -1176,13 +1192,13 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -1253,13 +1269,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -1275,7 +1291,7 @@
         <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1292,7 +1308,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1309,7 +1325,7 @@
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1325,7 +1341,9 @@
       <c r="D25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -1340,7 +1358,9 @@
       <c r="D26" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1358,89 +1378,97 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+      <c r="A28" s="9">
         <v>22</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>25</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="A33" s="9">
+        <v>26</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="1"/>
+      <c r="C33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1466,41 +1494,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="F3" s="18" t="s">
+      <c r="C3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="K3" s="18" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="P3" s="15" t="s">
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="P3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="17"/>
-      <c r="V3" s="18" t="s">
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="19"/>
+      <c r="V3" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
@@ -1921,16 +1949,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3851020-90A9-44B5-9DC2-1C613C04043C}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7726cb9a-a93a-4659-bc9a-e991ee8f575e"/>
+    <ds:schemaRef ds:uri="6a3f4802-9d90-487b-9ba2-7cd720365553"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="7726cb9a-a93a-4659-bc9a-e991ee8f575e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6a3f4802-9d90-487b-9ba2-7cd720365553"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated font style in content, created initial Product Review Model
</commit_message>
<xml_diff>
--- a/documentation/user_stories_models_v2.xlsx
+++ b/documentation/user_stories_models_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\608868804\OneDrive - BT Plc\Documents\Code_Institute\Milestone_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{3FFD8354-AF35-4189-879A-9D41E7FE4F0B}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{440A1350-F266-4908-B9D6-6E9FB687BFF0}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
   </bookViews>
   <sheets>
     <sheet name="User_Stories" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>User Story ID</t>
   </si>
@@ -332,12 +332,6 @@
     <t xml:space="preserve">rating </t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
     <t>review</t>
   </si>
   <si>
@@ -359,46 +353,49 @@
     <t>Order</t>
   </si>
   <si>
-    <t>Order/Bag Contents</t>
-  </si>
-  <si>
     <t>Complete - Special offers categories</t>
   </si>
   <si>
-    <t>Complete - visiible in header at all times</t>
-  </si>
-  <si>
     <t>Compelte</t>
   </si>
   <si>
     <t>Complete  - Bag app</t>
   </si>
   <si>
-    <t>Edit Shipping cost per country/continent</t>
-  </si>
-  <si>
-    <t>Option to change shipping cost depending on the location of the customer</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
     <t>stock</t>
   </si>
   <si>
-    <t>Can inventory field be added to product itself above</t>
-  </si>
-  <si>
     <t>Complete - Product App</t>
   </si>
   <si>
     <t>Update inventory number for item</t>
   </si>
   <si>
-    <t>Only show stock available, add warning when stock drops below a certain level</t>
-  </si>
-  <si>
     <t>Complete - Profile App</t>
+  </si>
+  <si>
+    <t>Complete  - Checkout App</t>
+  </si>
+  <si>
+    <t>View Inventory Status of a product</t>
+  </si>
+  <si>
+    <t>provide movitvation to purchase when stock be running low</t>
+  </si>
+  <si>
+    <t>Complete - Checkout</t>
+  </si>
+  <si>
+    <t>Complete - visible in header at all times</t>
+  </si>
+  <si>
+    <t>Add warning when stock drops below a certain level, only applow users to purchase items in stock</t>
+  </si>
+  <si>
+    <t>Added to Product Model</t>
   </si>
 </sst>
 </file>
@@ -607,7 +604,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -652,8 +649,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C557C4-B67B-4897-99C4-67C9935146BD}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,7 +982,7 @@
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1086,7 +1086,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1103,47 +1103,47 @@
         <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="20">
+        <v>6</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>60</v>
@@ -1151,16 +1151,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>60</v>
@@ -1168,16 +1168,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>60</v>
@@ -1185,16 +1185,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>60</v>
@@ -1202,322 +1202,326 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="E16" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>16</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="E28" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="9">
         <v>22</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="C29" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>23</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="E33" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
         <v>26</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="9" t="s">
+      <c r="C34" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="9">
-        <v>27</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1526,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2059F04D-4E8D-49F8-AE72-506C28E09033}">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11:J13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,18 +1543,19 @@
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5546875" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" s="15" t="s">
         <v>84</v>
       </c>
@@ -1561,25 +1566,26 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
       <c r="K3" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
       <c r="P3" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
       <c r="S3" s="19"/>
       <c r="V3" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA3" s="15"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>67</v>
       </c>
@@ -1622,19 +1628,22 @@
         <v>67</v>
       </c>
       <c r="W4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="X4" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1673,19 +1682,22 @@
         <v>1</v>
       </c>
       <c r="W5" s="1">
+        <v>1</v>
+      </c>
+      <c r="X5" s="1">
         <v>2</v>
       </c>
-      <c r="X5" s="1">
+      <c r="Y5" s="1">
         <v>3</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Z5" s="1">
         <v>4.2</v>
       </c>
-      <c r="Z5" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA5" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -1712,7 +1724,7 @@
       </c>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F7" s="1">
         <v>3</v>
       </c>
@@ -1723,35 +1735,35 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F11" s="15" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="I11" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="J11" s="20"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I11" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F12" s="8" t="s">
         <v>81</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
+        <v>99</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="I11:J13"/>
-    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="V3:AA3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="K3:M3"/>
@@ -1988,18 +2000,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2022,26 +2034,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3851020-90A9-44B5-9DC2-1C613C04043C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="6a3f4802-9d90-487b-9ba2-7cd720365553"/>
+    <ds:schemaRef ds:uri="7726cb9a-a93a-4659-bc9a-e991ee8f575e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3B3954-7716-4FAC-AC16-8DAEC6F571F0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3851020-90A9-44B5-9DC2-1C613C04043C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7726cb9a-a93a-4659-bc9a-e991ee8f575e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6a3f4802-9d90-487b-9ba2-7cd720365553"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
README - User stories intro complete
</commit_message>
<xml_diff>
--- a/documentation/user_stories_models_v2.xlsx
+++ b/documentation/user_stories_models_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\608868804\OneDrive - BT Plc\Documents\Code_Institute\Milestone_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{440A1350-F266-4908-B9D6-6E9FB687BFF0}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{92B8E0CA-BD3D-456D-B2A0-8A943F02ADFD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
   </bookViews>
   <sheets>
     <sheet name="User_Stories" sheetId="1" r:id="rId1"/>
@@ -31,42 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Meere,DJ,Damien,NQE33E R</author>
-  </authors>
-  <commentList>
-    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{990EB7B1-6556-45F0-9CF6-B4EB7527769C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Meere,DJ,Damien,NQE33E R:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-copy of product price (so completed order price won't change, if product price changes)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
   <si>
     <t>User Story ID</t>
   </si>
@@ -269,18 +235,6 @@
     <t>Complete - All_Products View</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>damien</t>
-  </si>
-  <si>
-    <t>dick</t>
-  </si>
-  <si>
     <t>prod_name</t>
   </si>
   <si>
@@ -302,33 +256,15 @@
     <t>comic</t>
   </si>
   <si>
-    <t>Order_num</t>
-  </si>
-  <si>
     <t>user_FK</t>
   </si>
   <si>
-    <t>order_FK</t>
-  </si>
-  <si>
     <t>prod_FK</t>
   </si>
   <si>
-    <t>00001</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
     <t xml:space="preserve">rating </t>
   </si>
   <si>
@@ -350,9 +286,6 @@
     <t>Data Models</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>Complete - Special offers categories</t>
   </si>
   <si>
@@ -362,12 +295,6 @@
     <t>Complete  - Bag app</t>
   </si>
   <si>
-    <t>Inventory</t>
-  </si>
-  <si>
-    <t>stock</t>
-  </si>
-  <si>
     <t>Complete - Product App</t>
   </si>
   <si>
@@ -395,14 +322,74 @@
     <t>Add warning when stock drops below a certain level, only applow users to purchase items in stock</t>
   </si>
   <si>
-    <t>Added to Product Model</t>
+    <t>Mailing List</t>
+  </si>
+  <si>
+    <t>Enable the user to sign up or opt out of the mialing list (both anonymous and sign up users</t>
+  </si>
+  <si>
+    <t>Complete Products + Profile</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>has_sizes</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>image_URL</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>stock_level</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Stock level and rating based on user input</t>
+  </si>
+  <si>
+    <t>review_id</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>linked to Product through foreign key. Reviews can only be created via the Order page.</t>
+  </si>
+  <si>
+    <t>Subscriber List</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>subscriber _ID</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>User can subscribe theough the home back link or through their individual profule update page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,20 +422,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,12 +463,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,26 +575,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,31 +609,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -971,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C557C4-B67B-4897-99C4-67C9935146BD}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,19 +972,19 @@
       <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1086,7 +1062,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1103,24 +1079,24 @@
         <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>106</v>
+      <c r="C9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1133,16 +1109,16 @@
       <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1150,16 +1126,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1167,16 +1143,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1184,16 +1160,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>9</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1201,16 +1177,16 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1218,47 +1194,47 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>11</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="2">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>12</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -1268,13 +1244,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1285,13 +1261,13 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1302,40 +1278,40 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>16</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1345,13 +1321,13 @@
         <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1362,13 +1338,13 @@
         <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1379,13 +1355,13 @@
         <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1396,13 +1372,13 @@
         <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1413,55 +1389,57 @@
         <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>22</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
-        <v>22</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="E29" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="C30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>23</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
@@ -1471,13 +1449,13 @@
         <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1488,40 +1466,57 @@
         <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
-        <v>26</v>
-      </c>
-      <c r="B34" s="3" t="s">
+      <c r="E34" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>27</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>103</v>
+      <c r="C35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A31:E31"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1529,250 +1524,268 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2059F04D-4E8D-49F8-AE72-506C28E09033}">
-  <dimension ref="A1:AA13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2059F04D-4E8D-49F8-AE72-506C28E09033}">
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" customWidth="1"/>
     <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
     <col min="23" max="23" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="15"/>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F3" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="K3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="P3" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19"/>
-      <c r="V3" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="W4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA4" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="I4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="R5" s="1">
-        <v>3</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="V5" s="1">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1">
-        <v>1</v>
-      </c>
-      <c r="X5" s="1">
-        <v>2</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>3</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F6" s="1">
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P6" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1">
-        <v>2</v>
-      </c>
-      <c r="S6" s="1"/>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F7" s="1">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="M11" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="F11" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="I11" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="F12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
+      <c r="K12" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F13" s="1">
+        <v>1232432421</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F16" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="I16" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F17" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F18" s="1">
+        <v>3243245325</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J13"/>
-    <mergeCell ref="V3:AA3"/>
+  <mergeCells count="7">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:P3"/>
+    <mergeCell ref="R4:T5"/>
+    <mergeCell ref="M11:O14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I16:K18"/>
+    <mergeCell ref="F11:K11"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G18" r:id="rId1" xr:uid="{0E6E72C9-7EEF-44C5-97EE-05987144B4FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2036,16 +2049,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3851020-90A9-44B5-9DC2-1C613C04043C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="6a3f4802-9d90-487b-9ba2-7cd720365553"/>
     <ds:schemaRef ds:uri="7726cb9a-a93a-4659-bc9a-e991ee8f575e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
README - User Stories - ID 17
</commit_message>
<xml_diff>
--- a/documentation/user_stories_models_v2.xlsx
+++ b/documentation/user_stories_models_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\608868804\OneDrive - BT Plc\Documents\Code_Institute\Milestone_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{92B8E0CA-BD3D-456D-B2A0-8A943F02ADFD}"/>
+  <xr:revisionPtr revIDLastSave="203" documentId="8_{2129E99A-7339-4C62-8D64-1FF9992E20A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9CBE2A95-FFC7-4362-8682-0C72D159A23A}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B29801E3-267D-4C77-85E0-EDC3ADC41264}"/>
   </bookViews>
   <sheets>
     <sheet name="User_Stories" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>User Story ID</t>
   </si>
@@ -430,7 +430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +463,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,7 +587,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -630,6 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -949,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C557C4-B67B-4897-99C4-67C9935146BD}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:E31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1143,21 +1150,19 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="22">
         <v>8</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="E13" s="22"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">

</xml_diff>